<commit_message>
updated results of auto testing
</commit_message>
<xml_diff>
--- a/robots/claymore/AutoChar.xlsx
+++ b/robots/claymore/AutoChar.xlsx
@@ -8,15 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\ButchGriffin\src\robotdev\robots\claymore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3DB3E522-D957-46C4-9B5F-71C37D877B8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{62CA2ABD-BB6C-47FF-8776-E42874E27932}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12180" activeTab="3" xr2:uid="{A940171D-E55F-4BC9-9086-8C3698129B04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12180" tabRatio="705" xr2:uid="{A940171D-E55F-4BC9-9086-8C3698129B04}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Collector" sheetId="3" r:id="rId2"/>
-    <sheet name="CenterTwoSwitch" sheetId="2" r:id="rId3"/>
-    <sheet name="CenterScaleLeft" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="50">
   <si>
     <t>Switch</t>
   </si>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>Cross line</t>
-  </si>
-  <si>
-    <t>Time</t>
   </si>
   <si>
     <t>Score in left switch from front
@@ -144,64 +138,61 @@
     <t>Left/Right</t>
   </si>
   <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>1st</t>
-  </si>
-  <si>
-    <t>2nd</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Did not do timed run</t>
-  </si>
-  <si>
-    <t>Sitting at switch with cube in hand</t>
-  </si>
-  <si>
-    <t>Lost Cubes</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Turned to pile ready to collect 3rd cube</t>
-  </si>
-  <si>
-    <t>Dropped 2, but did not get turned</t>
-  </si>
-  <si>
     <t>5/5</t>
   </si>
   <si>
     <t>4/5</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>CenterTwoSwitch</t>
-  </si>
-  <si>
-    <t>CenterScaleLeft</t>
-  </si>
-  <si>
-    <t>Coasted into final position without final turn</t>
+    <t>0/5</t>
+  </si>
+  <si>
+    <t>5/6</t>
+  </si>
+  <si>
+    <t>3/5</t>
+  </si>
+  <si>
+    <t>1/5</t>
+  </si>
+  <si>
+    <t>2/2</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>It worked reliably, but did not quite get to the far left.  It was close, should consider 100% successful.</t>
+  </si>
+  <si>
+    <t>Second cube is right at the end of time</t>
+  </si>
+  <si>
+    <t>Never use in competition</t>
+  </si>
+  <si>
+    <t>Works</t>
+  </si>
+  <si>
+    <t>Adjusted angle and eject speed while running, should work a little better than the data indicates.</t>
+  </si>
+  <si>
+    <t>The miss was the turn to collect the second cube stalled.</t>
+  </si>
+  <si>
+    <t>Struggled with turn stalling when going to collect second cube, same turns as scale/scale which we improved</t>
+  </si>
+  <si>
+    <t>Works but is right at the edge of time</t>
+  </si>
+  <si>
+    <t>Adjusted eject speed for miss on first cube, the angle on the 2nd cube collect was the miss on the second cube.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -247,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -372,11 +363,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -395,9 +423,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -414,6 +439,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -423,12 +470,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{696152FE-01B2-4CCD-BEE2-5F2C104B4BF0}">
-  <dimension ref="B1:L42"/>
+  <dimension ref="B1:J42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,41 +796,41 @@
     <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" customWidth="1"/>
     <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="21"/>
-      <c r="C2" s="22" t="s">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="18"/>
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="24" t="s">
+      <c r="I2" s="21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
-        <v>23</v>
+      <c r="J2" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="38" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="11">
         <v>0</v>
@@ -809,13 +850,15 @@
       <c r="H3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
+      <c r="J3" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="39"/>
       <c r="C4" s="2">
         <v>0</v>
       </c>
@@ -834,13 +877,15 @@
       <c r="H4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="26"/>
+      <c r="J4" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="39"/>
       <c r="C5" s="2">
         <v>0</v>
       </c>
@@ -859,13 +904,15 @@
       <c r="H5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="27"/>
+      <c r="J5" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="40"/>
       <c r="C6" s="8">
         <v>0</v>
       </c>
@@ -884,14 +931,15 @@
       <c r="H6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="26" t="s">
+      <c r="J6" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B7" s="39" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1">
@@ -906,17 +954,21 @@
       <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="26"/>
+      <c r="G7" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="39"/>
       <c r="C8" s="1">
         <v>1</v>
       </c>
@@ -929,15 +981,21 @@
       <c r="F8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="26"/>
+      <c r="G8" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="39"/>
       <c r="C9" s="1">
         <v>1</v>
       </c>
@@ -950,15 +1008,21 @@
       <c r="F9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="26"/>
+      <c r="G9" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="39"/>
       <c r="C10" s="1">
         <v>1</v>
       </c>
@@ -971,21 +1035,21 @@
       <c r="F10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="26"/>
+      <c r="G10" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="39"/>
       <c r="C11" s="2">
         <v>2</v>
       </c>
@@ -998,15 +1062,21 @@
       <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B12" s="26"/>
+      <c r="G11" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="39"/>
       <c r="C12" s="2">
         <v>2</v>
       </c>
@@ -1019,15 +1089,21 @@
       <c r="F12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B13" s="26"/>
+      <c r="G12" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="39"/>
       <c r="C13" s="2">
         <v>2</v>
       </c>
@@ -1040,15 +1116,21 @@
       <c r="F13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="26"/>
+      <c r="G13" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="39"/>
       <c r="C14" s="2">
         <v>2</v>
       </c>
@@ -1061,16 +1143,22 @@
       <c r="F14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B15" s="25" t="s">
-        <v>24</v>
+      <c r="G14" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="38" t="s">
+        <v>23</v>
       </c>
       <c r="C15" s="3">
         <v>3</v>
@@ -1084,15 +1172,21 @@
       <c r="F15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="26"/>
+      <c r="G15" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="39"/>
       <c r="C16" s="1">
         <v>3</v>
       </c>
@@ -1105,15 +1199,21 @@
       <c r="F16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="5" t="s">
-        <v>19</v>
+      <c r="G16" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B17" s="26"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="1">
         <v>3</v>
       </c>
@@ -1126,15 +1226,21 @@
       <c r="F17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="5" t="s">
-        <v>21</v>
+      <c r="G17" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="26"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="1">
         <v>3</v>
       </c>
@@ -1147,15 +1253,21 @@
       <c r="F18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="5" t="s">
+      <c r="G18" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="J18" s="31" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="26"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="2">
         <v>4</v>
       </c>
@@ -1168,15 +1280,21 @@
       <c r="F19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="6" t="s">
-        <v>19</v>
+      <c r="G19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="26"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="2">
         <v>4</v>
       </c>
@@ -1189,15 +1307,21 @@
       <c r="F20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="6" t="s">
-        <v>19</v>
+      <c r="G20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="31" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B21" s="26"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="2">
         <v>4</v>
       </c>
@@ -1210,15 +1334,21 @@
       <c r="F21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="18" t="s">
-        <v>21</v>
+      <c r="G21" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="26"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="2">
         <v>4</v>
       </c>
@@ -1231,15 +1361,21 @@
       <c r="F22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="6" t="s">
+      <c r="G22" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="J22" s="31" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="26"/>
+      <c r="B23" s="39"/>
       <c r="C23" s="1">
         <v>5</v>
       </c>
@@ -1252,15 +1388,21 @@
       <c r="F23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="7" t="s">
+      <c r="G23" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="J23" s="31" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="24" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B24" s="26"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="1">
         <v>5</v>
       </c>
@@ -1273,15 +1415,21 @@
       <c r="F24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="19" t="s">
-        <v>22</v>
+      <c r="G24" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="31" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="26"/>
+      <c r="B25" s="39"/>
       <c r="C25" s="1">
         <v>5</v>
       </c>
@@ -1294,15 +1442,21 @@
       <c r="F25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="7" t="s">
-        <v>20</v>
+      <c r="G25" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="31" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B26" s="26"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="1">
         <v>5</v>
       </c>
@@ -1315,15 +1469,21 @@
       <c r="F26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="19" t="s">
-        <v>22</v>
+      <c r="G26" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="31" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="26"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="2">
         <v>6</v>
       </c>
@@ -1336,15 +1496,21 @@
       <c r="F27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="6" t="s">
+      <c r="G27" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="J27" s="31" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="28" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B28" s="26"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="2">
         <v>6</v>
       </c>
@@ -1357,15 +1523,21 @@
       <c r="F28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="18" t="s">
-        <v>22</v>
+      <c r="G28" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" s="31" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="26"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="2">
         <v>6</v>
       </c>
@@ -1378,15 +1550,21 @@
       <c r="F29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="6" t="s">
-        <v>20</v>
+      <c r="G29" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="27"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="8">
         <v>6</v>
       </c>
@@ -1399,16 +1577,22 @@
       <c r="F30" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="9" t="s">
-        <v>20</v>
+      <c r="G30" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B31" s="25" t="s">
-        <v>25</v>
+      <c r="B31" s="38" t="s">
+        <v>24</v>
       </c>
       <c r="C31" s="3">
         <v>7</v>
@@ -1422,15 +1606,21 @@
       <c r="F31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="20" t="s">
-        <v>29</v>
+      <c r="G31" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="I31" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" s="33" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="26"/>
+      <c r="B32" s="39"/>
       <c r="C32" s="1">
         <v>7</v>
       </c>
@@ -1443,15 +1633,21 @@
       <c r="F32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="7" t="s">
-        <v>30</v>
+      <c r="G32" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32" s="31" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B33" s="26"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="1">
         <v>7</v>
       </c>
@@ -1464,15 +1660,21 @@
       <c r="F33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="5" t="s">
-        <v>21</v>
+      <c r="G33" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" s="31" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="26"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="1">
         <v>7</v>
       </c>
@@ -1485,15 +1687,21 @@
       <c r="F34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="7" t="s">
-        <v>30</v>
+      <c r="G34" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J34" s="31" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="26"/>
+      <c r="B35" s="39"/>
       <c r="C35" s="2">
         <v>8</v>
       </c>
@@ -1506,15 +1714,21 @@
       <c r="F35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="6" t="s">
-        <v>31</v>
+      <c r="G35" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35" s="31" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B36" s="26"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="2">
         <v>8</v>
       </c>
@@ -1527,15 +1741,21 @@
       <c r="F36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="18" t="s">
-        <v>22</v>
+      <c r="G36" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" s="31" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="26"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="2">
         <v>8</v>
       </c>
@@ -1548,15 +1768,17 @@
       <c r="F37" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="6" t="s">
-        <v>31</v>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J37" s="31" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="27"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="8">
         <v>8</v>
       </c>
@@ -1569,22 +1791,28 @@
       <c r="F38" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="18" t="s">
-        <v>32</v>
+      <c r="G38" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J38" s="32" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="25" t="s">
-        <v>28</v>
+      <c r="B39" s="38" t="s">
+        <v>27</v>
       </c>
       <c r="C39" s="3">
         <v>9</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>4</v>
@@ -1592,20 +1820,26 @@
       <c r="F39" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="14"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="10" t="s">
+      <c r="G39" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I39" s="10" t="s">
         <v>14</v>
       </c>
+      <c r="J39" s="31" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="26"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="1">
         <v>9</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>4</v>
@@ -1613,20 +1847,26 @@
       <c r="F40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G40" s="15"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="7" t="s">
+      <c r="G40" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I40" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="J40" s="31" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B41" s="26"/>
+      <c r="B41" s="39"/>
       <c r="C41" s="1">
         <v>9</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>6</v>
@@ -1634,20 +1874,26 @@
       <c r="F41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="15"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="7" t="s">
+      <c r="G41" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H41" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="J41" s="31" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="42" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="27"/>
+      <c r="B42" s="40"/>
       <c r="C42" s="13">
         <v>9</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>6</v>
@@ -1655,11 +1901,17 @@
       <c r="F42" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G42" s="16"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="17" t="s">
+      <c r="G42" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="H42" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="I42" s="14" t="s">
         <v>14</v>
+      </c>
+      <c r="J42" s="32" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1673,258 +1925,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317688DF-3A0D-4FC8-B92E-66190F801CFB}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE02A02-A609-4912-8E2E-0283D983047C}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="28.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="28">
-        <v>15.4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="28">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="28">
-        <v>15.6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="28">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="28">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACAD84F8-FDFD-4BB7-B825-ACCE7CA3FC83}">
-  <dimension ref="A1:E1048576"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="54.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="28">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="28">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="28">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="28"/>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="28"/>
-    </row>
-    <row r="1048576" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B1048576" s="28"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated automodes testing spreadsheet
</commit_message>
<xml_diff>
--- a/robots/claymore/AutoChar.xlsx
+++ b/robots/claymore/AutoChar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\ButchGriffin\src\robotdev\robots\claymore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin\home\ButchGriffin\src\robotdev\robots\claymore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{62CA2ABD-BB6C-47FF-8776-E42874E27932}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8ADDE6-4293-4FA1-B61E-33C511B27D3E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="12180" tabRatio="705" xr2:uid="{A940171D-E55F-4BC9-9086-8C3698129B04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="12180" tabRatio="705" xr2:uid="{A940171D-E55F-4BC9-9086-8C3698129B04}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -784,24 +784,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{696152FE-01B2-4CCD-BEE2-5F2C104B4BF0}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="L2" sqref="L2:L42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" customWidth="1"/>
-    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="2" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="18"/>
       <c r="C2" s="19" t="s">
         <v>0</v>
@@ -828,7 +831,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="38" t="s">
         <v>22</v>
       </c>
@@ -857,7 +860,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="39"/>
       <c r="C4" s="2">
         <v>0</v>
@@ -884,7 +887,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="39"/>
       <c r="C5" s="2">
         <v>0</v>
@@ -911,7 +914,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="40"/>
       <c r="C6" s="8">
         <v>0</v>
@@ -938,7 +941,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B7" s="39" t="s">
         <v>11</v>
       </c>
@@ -967,7 +970,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B8" s="39"/>
       <c r="C8" s="1">
         <v>1</v>
@@ -994,7 +997,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="39"/>
       <c r="C9" s="1">
         <v>1</v>
@@ -1021,7 +1024,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="39"/>
       <c r="C10" s="1">
         <v>1</v>
@@ -1048,7 +1051,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B11" s="39"/>
       <c r="C11" s="2">
         <v>2</v>
@@ -1075,7 +1078,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B12" s="39"/>
       <c r="C12" s="2">
         <v>2</v>
@@ -1102,7 +1105,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B13" s="39"/>
       <c r="C13" s="2">
         <v>2</v>
@@ -1129,7 +1132,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="39"/>
       <c r="C14" s="2">
         <v>2</v>
@@ -1156,7 +1159,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B15" s="38" t="s">
         <v>23</v>
       </c>
@@ -1185,7 +1188,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="39"/>
       <c r="C16" s="1">
         <v>3</v>
@@ -1212,7 +1215,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B17" s="39"/>
       <c r="C17" s="1">
         <v>3</v>
@@ -1239,7 +1242,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="39"/>
       <c r="C18" s="1">
         <v>3</v>
@@ -1266,7 +1269,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="39"/>
       <c r="C19" s="2">
         <v>4</v>
@@ -1293,7 +1296,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="39"/>
       <c r="C20" s="2">
         <v>4</v>
@@ -1320,7 +1323,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B21" s="39"/>
       <c r="C21" s="2">
         <v>4</v>
@@ -1347,7 +1350,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22" s="39"/>
       <c r="C22" s="2">
         <v>4</v>
@@ -1374,7 +1377,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B23" s="39"/>
       <c r="C23" s="1">
         <v>5</v>
@@ -1401,7 +1404,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B24" s="39"/>
       <c r="C24" s="1">
         <v>5</v>
@@ -1428,7 +1431,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B25" s="39"/>
       <c r="C25" s="1">
         <v>5</v>
@@ -1455,7 +1458,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B26" s="39"/>
       <c r="C26" s="1">
         <v>5</v>
@@ -1482,7 +1485,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" s="39"/>
       <c r="C27" s="2">
         <v>6</v>
@@ -1509,7 +1512,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B28" s="39"/>
       <c r="C28" s="2">
         <v>6</v>
@@ -1536,7 +1539,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B29" s="39"/>
       <c r="C29" s="2">
         <v>6</v>
@@ -1563,7 +1566,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="40"/>
       <c r="C30" s="8">
         <v>6</v>
@@ -1590,7 +1593,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B31" s="38" t="s">
         <v>24</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B32" s="39"/>
       <c r="C32" s="1">
         <v>7</v>
@@ -1646,7 +1649,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B33" s="39"/>
       <c r="C33" s="1">
         <v>7</v>
@@ -1673,7 +1676,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B34" s="39"/>
       <c r="C34" s="1">
         <v>7</v>
@@ -1700,7 +1703,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" s="39"/>
       <c r="C35" s="2">
         <v>8</v>
@@ -1727,7 +1730,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B36" s="39"/>
       <c r="C36" s="2">
         <v>8</v>
@@ -1754,7 +1757,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37" s="39"/>
       <c r="C37" s="2">
         <v>8</v>
@@ -1777,7 +1780,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B38" s="40"/>
       <c r="C38" s="8">
         <v>8</v>
@@ -1804,7 +1807,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B39" s="38" t="s">
         <v>27</v>
       </c>
@@ -1833,7 +1836,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B40" s="39"/>
       <c r="C40" s="1">
         <v>9</v>
@@ -1860,7 +1863,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B41" s="39"/>
       <c r="C41" s="1">
         <v>9</v>
@@ -1887,7 +1890,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B42" s="40"/>
       <c r="C42" s="13">
         <v>9</v>
@@ -1922,7 +1925,7 @@
     <mergeCell ref="B31:B38"/>
     <mergeCell ref="B39:B42"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0" footer="0"/>
+  <pageSetup scale="69" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>